<commit_message>
Add more readable formatting
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -80,11 +80,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="h:mm;@"/>
-    <numFmt numFmtId="166" formatCode="[h]:mm:ss"/>
-    <numFmt numFmtId="167" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="165" formatCode="ddd&quot;, &quot;d/\ mmm\ yy"/>
+    <numFmt numFmtId="166" formatCode="hh:mm"/>
+    <numFmt numFmtId="167" formatCode="[h]:mm:ss"/>
+    <numFmt numFmtId="168" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -250,7 +251,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -295,11 +296,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -307,7 +316,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -323,7 +332,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -331,11 +340,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -433,10 +442,10 @@
   <dimension ref="A1:AMJ41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9:F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.47265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="1" width="14.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="13.67"/>
@@ -554,11 +563,11 @@
     </row>
     <row r="9" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12" t="n">
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="14" t="n">
         <f aca="false">SUM(D9-C9-E9)</f>
         <v>0</v>
       </c>
@@ -568,11 +577,11 @@
     </row>
     <row r="10" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12" t="n">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="14" t="n">
         <f aca="false">SUM(D10-C10-E10)</f>
         <v>0</v>
       </c>
@@ -582,11 +591,11 @@
     </row>
     <row r="11" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12" t="n">
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="14" t="n">
         <f aca="false">SUM(D11-C11-E11)</f>
         <v>0</v>
       </c>
@@ -596,11 +605,11 @@
     </row>
     <row r="12" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12" t="n">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="14" t="n">
         <f aca="false">SUM(D12-C12-E12)</f>
         <v>0</v>
       </c>
@@ -610,11 +619,11 @@
     </row>
     <row r="13" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12" t="n">
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="14" t="n">
         <f aca="false">SUM(D13-C13-E13)</f>
         <v>0</v>
       </c>
@@ -624,11 +633,11 @@
     </row>
     <row r="14" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12" t="n">
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="14" t="n">
         <f aca="false">SUM(D14-C14-E14)</f>
         <v>0</v>
       </c>
@@ -638,11 +647,11 @@
     </row>
     <row r="15" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12" t="n">
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="14" t="n">
         <f aca="false">SUM(D15-C15-E15)</f>
         <v>0</v>
       </c>
@@ -652,11 +661,11 @@
     </row>
     <row r="16" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="12" t="n">
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="14" t="n">
         <f aca="false">SUM(D16-C16-E16)</f>
         <v>0</v>
       </c>
@@ -666,11 +675,11 @@
     </row>
     <row r="17" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="12" t="n">
+      <c r="B17" s="12"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="14" t="n">
         <f aca="false">SUM(D17-C17-E17)</f>
         <v>0</v>
       </c>
@@ -680,11 +689,11 @@
     </row>
     <row r="18" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="12" t="n">
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="14" t="n">
         <f aca="false">SUM(D18-C18-E18)</f>
         <v>0</v>
       </c>
@@ -694,11 +703,11 @@
     </row>
     <row r="19" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="12" t="n">
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="14" t="n">
         <f aca="false">SUM(D19-C19-E19)</f>
         <v>0</v>
       </c>
@@ -708,11 +717,11 @@
     </row>
     <row r="20" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="12" t="n">
+      <c r="B20" s="12"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="14" t="n">
         <f aca="false">SUM(D20-C20-E20)</f>
         <v>0</v>
       </c>
@@ -722,11 +731,11 @@
     </row>
     <row r="21" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="12" t="n">
+      <c r="B21" s="12"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="14" t="n">
         <f aca="false">SUM(D21-C21-E21)</f>
         <v>0</v>
       </c>
@@ -736,11 +745,11 @@
     </row>
     <row r="22" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="12" t="n">
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="14" t="n">
         <f aca="false">SUM(D22-C22-E22)</f>
         <v>0</v>
       </c>
@@ -750,11 +759,11 @@
     </row>
     <row r="23" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="12" t="n">
+      <c r="B23" s="12"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="14" t="n">
         <f aca="false">SUM(D23-C23-E23)</f>
         <v>0</v>
       </c>
@@ -764,11 +773,11 @@
     </row>
     <row r="24" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="12" t="n">
+      <c r="B24" s="12"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="14" t="n">
         <f aca="false">SUM(D24-C24-E24)</f>
         <v>0</v>
       </c>
@@ -778,11 +787,11 @@
     </row>
     <row r="25" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="12" t="n">
+      <c r="B25" s="12"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="14" t="n">
         <f aca="false">SUM(D25-C25-E25)</f>
         <v>0</v>
       </c>
@@ -792,11 +801,11 @@
     </row>
     <row r="26" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="12" t="n">
+      <c r="B26" s="12"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="14" t="n">
         <f aca="false">SUM(D26-C26-E26)</f>
         <v>0</v>
       </c>
@@ -806,11 +815,11 @@
     </row>
     <row r="27" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="12" t="n">
+      <c r="B27" s="12"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="14" t="n">
         <f aca="false">SUM(D27-C27-E27)</f>
         <v>0</v>
       </c>
@@ -820,11 +829,11 @@
     </row>
     <row r="28" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="12" t="n">
+      <c r="B28" s="12"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="14" t="n">
         <f aca="false">SUM(D28-C28-E28)</f>
         <v>0</v>
       </c>
@@ -834,11 +843,11 @@
     </row>
     <row r="29" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="12" t="n">
+      <c r="B29" s="12"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="14" t="n">
         <f aca="false">SUM(D29-C29-E29)</f>
         <v>0</v>
       </c>
@@ -848,11 +857,11 @@
     </row>
     <row r="30" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="12" t="n">
+      <c r="B30" s="12"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="14" t="n">
         <f aca="false">SUM(D30-C30-E30)</f>
         <v>0</v>
       </c>
@@ -862,11 +871,11 @@
     </row>
     <row r="31" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="12" t="n">
+      <c r="B31" s="12"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="14" t="n">
         <f aca="false">SUM(D31-C31-E31)</f>
         <v>0</v>
       </c>
@@ -876,11 +885,11 @@
     </row>
     <row r="32" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="12" t="n">
+      <c r="B32" s="12"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="14" t="n">
         <f aca="false">SUM(D32-C32-E32)</f>
         <v>0</v>
       </c>
@@ -888,29 +897,29 @@
       <c r="H32" s="6"/>
       <c r="AMJ32" s="0"/>
     </row>
-    <row r="33" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="13" t="s">
+    <row r="33" s="18" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="14" t="n">
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="16" t="n">
         <f aca="false">SUM(F9:F32)</f>
         <v>0</v>
       </c>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
       <c r="AMJ33" s="0"/>
     </row>
     <row r="34" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="17"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="18"/>
+      <c r="A34" s="19"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="20"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
       <c r="AMJ34" s="0"/>
@@ -927,27 +936,27 @@
       <c r="AMJ35" s="0"/>
     </row>
     <row r="36" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="19"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="20"/>
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="22"/>
       <c r="D36" s="6"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
       <c r="AMJ36" s="0"/>
     </row>
     <row r="37" s="7" customFormat="true" ht="15.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="22" t="s">
+      <c r="A37" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="24"/>
       <c r="D37" s="6"/>
-      <c r="E37" s="22" t="s">
+      <c r="E37" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="F37" s="22"/>
+      <c r="F37" s="24"/>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
       <c r="AMJ37" s="0"/>
@@ -964,27 +973,27 @@
       <c r="AMJ38" s="0"/>
     </row>
     <row r="39" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="19"/>
-      <c r="B39" s="19"/>
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
       <c r="AMJ39" s="0"/>
     </row>
     <row r="40" s="7" customFormat="true" ht="15.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="22" t="s">
+      <c r="A40" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B40" s="22"/>
-      <c r="C40" s="22"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="24"/>
       <c r="D40" s="6"/>
-      <c r="E40" s="22" t="s">
+      <c r="E40" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="F40" s="22"/>
+      <c r="F40" s="24"/>
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
       <c r="AMJ40" s="0"/>

</xml_diff>